<commit_message>
support for multiple tables in one sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/test-todos.xlsx
+++ b/src/test/resources/test-todos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m_plo\Documents\Projects\reflective-excel\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CE95B2A-1935-44CD-89C9-866C41E32DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C50807C1-02C2-4134-8D65-4DC655C63735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Description</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>write this library</t>
+  </si>
+  <si>
+    <t>dummy val</t>
   </si>
 </sst>
 </file>
@@ -379,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -390,9 +393,10 @@
     <col min="1" max="1" width="24.5546875" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -403,7 +407,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -414,7 +418,7 @@
         <v>45272</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -424,8 +428,11 @@
       <c r="C3" s="2">
         <v>45273</v>
       </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>

</xml_diff>